<commit_message>
Se agrega el mensaje main
</commit_message>
<xml_diff>
--- a/Actas/02_Historia_Usuario.xlsx
+++ b/Actas/02_Historia_Usuario.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\CICLO 3 PROYECTO\Actas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{564835C1-F48E-43F7-A790-D6EACE52613F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111D34F1-52B5-4546-B132-E669E4903793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de usuario" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de usuario'!$A$1:$F$96</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -238,6 +241,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -254,23 +263,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="12" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,8 +495,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:F99"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A41" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -503,54 +506,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="19">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
+      <c r="C4" s="16"/>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -575,7 +578,7 @@
       <c r="D7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="17">
         <v>44317</v>
       </c>
       <c r="F7" s="11"/>
@@ -591,7 +594,7 @@
       <c r="D8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="22">
         <v>6.5</v>
       </c>
       <c r="F8" s="11"/>
@@ -607,152 +610,152 @@
       <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="22">
         <v>8</v>
       </c>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
     </row>
     <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="19">
         <v>2</v>
       </c>
-      <c r="C24" s="14"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -777,7 +780,7 @@
       <c r="D27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="17">
         <v>44256</v>
       </c>
       <c r="F27" s="11"/>
@@ -815,146 +818,146 @@
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="19">
         <v>1</v>
       </c>
-      <c r="C44" s="14"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="14"/>
+      <c r="F44" s="16"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
@@ -979,7 +982,7 @@
       <c r="D47" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="15">
+      <c r="E47" s="17">
         <v>44256</v>
       </c>
       <c r="F47" s="11"/>
@@ -1017,146 +1020,146 @@
       <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
+      <c r="B50" s="21"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="23"/>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="23"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="23"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
+      <c r="A62" s="16"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B64" s="17">
+      <c r="B64" s="19">
         <v>1</v>
       </c>
-      <c r="C64" s="14"/>
+      <c r="C64" s="16"/>
       <c r="D64" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E64" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F64" s="14"/>
+      <c r="F64" s="16"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="13"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
@@ -1181,7 +1184,7 @@
       <c r="D67" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E67" s="15">
+      <c r="E67" s="17">
         <v>44256</v>
       </c>
       <c r="F67" s="11"/>
@@ -1219,146 +1222,146 @@
       <c r="F69" s="11"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B70" s="23"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="23"/>
-      <c r="E70" s="23"/>
-      <c r="F70" s="23"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="23"/>
-      <c r="B71" s="23"/>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23"/>
-      <c r="F71" s="23"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="23"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="23"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
-      <c r="F72" s="23"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="23"/>
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23"/>
-      <c r="C74" s="23"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
-      <c r="F74" s="23"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="12" t="s">
+      <c r="A75" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="12"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="13"/>
-      <c r="B80" s="14"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
     </row>
     <row r="81" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="14"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
+      <c r="D81" s="16"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
     </row>
     <row r="82" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="14"/>
-      <c r="B82" s="14"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
     </row>
     <row r="83" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="13"/>
-      <c r="B83" s="14"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
+      <c r="A83" s="15"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
     </row>
     <row r="84" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B84" s="17">
+      <c r="B84" s="19">
         <v>1</v>
       </c>
-      <c r="C84" s="14"/>
+      <c r="C84" s="16"/>
       <c r="D84" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E84" s="17" t="s">
+      <c r="E84" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F84" s="14"/>
+      <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="13"/>
-      <c r="B85" s="14"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
+      <c r="A85" s="15"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
@@ -1383,7 +1386,7 @@
       <c r="D87" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E87" s="15">
+      <c r="E87" s="17">
         <v>44256</v>
       </c>
       <c r="F87" s="11"/>
@@ -1421,135 +1424,122 @@
       <c r="F89" s="11"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="20" t="s">
+      <c r="A90" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="21"/>
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="21"/>
-      <c r="E91" s="21"/>
-      <c r="F91" s="21"/>
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="21"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="21"/>
-      <c r="F92" s="21"/>
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="21"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
-      <c r="E93" s="21"/>
-      <c r="F93" s="21"/>
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="21"/>
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="21"/>
-      <c r="E94" s="21"/>
-      <c r="F94" s="21"/>
+      <c r="A94" s="13"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B95" s="12"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="12"/>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
+      <c r="A96" s="14"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="12"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="12"/>
-      <c r="E97" s="12"/>
-      <c r="F97" s="12"/>
+      <c r="A97" s="14"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="12"/>
-      <c r="B98" s="12"/>
-      <c r="C98" s="12"/>
-      <c r="D98" s="12"/>
-      <c r="E98" s="12"/>
-      <c r="F98" s="12"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="12"/>
-      <c r="B99" s="12"/>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
+      <c r="A99" s="14"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="13"/>
-      <c r="B100" s="14"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14"/>
+      <c r="A100" s="15"/>
+      <c r="B100" s="16"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16"/>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="A90:F94"/>
-    <mergeCell ref="A95:F99"/>
-    <mergeCell ref="A100:F100"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="E87:F87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="E88:F88"/>
-    <mergeCell ref="A81:F82"/>
-    <mergeCell ref="A83:F83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="A70:F74"/>
-    <mergeCell ref="A75:F79"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="A61:F62"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="A21:F22"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="A50:F54"/>
+    <mergeCell ref="A55:F59"/>
+    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="A41:F42"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="E8:F8"/>
@@ -1566,31 +1556,47 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A41:F42"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="A50:F54"/>
-    <mergeCell ref="A55:F59"/>
-    <mergeCell ref="A60:F60"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="A21:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A61:F62"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="A65:F65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="A70:F74"/>
+    <mergeCell ref="A75:F79"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A81:F82"/>
+    <mergeCell ref="A83:F83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="E87:F87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="E88:F88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="E89:F89"/>
+    <mergeCell ref="A90:F94"/>
+    <mergeCell ref="A95:F99"/>
+    <mergeCell ref="A100:F100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="85" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="40" max="5" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>